<commit_message>
[UPDATE] Budget Return, All, Years and Duplicate
</commit_message>
<xml_diff>
--- a/uploads/excel/RKAP Tempalate Fix.xlsx
+++ b/uploads/excel/RKAP Tempalate Fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Magang\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7449FC0-7E6B-4E93-8648-6D49D0DC625E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0C7CF8-DBC2-4B42-ACDE-9C09A150F199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9795" yWindow="2910" windowWidth="14205" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rkap" sheetId="1" r:id="rId1"/>
@@ -2135,8 +2135,8 @@
   </sheetPr>
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2193,7 +2193,7 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
@@ -2340,7 +2340,7 @@
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>15</v>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>15</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>15</v>
@@ -2732,7 +2732,7 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
@@ -2781,7 +2781,7 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
@@ -2828,7 +2828,7 @@
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>16</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>16</v>
@@ -3063,7 +3063,7 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>16</v>
@@ -3110,7 +3110,7 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>16</v>
@@ -3157,7 +3157,7 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>16</v>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>16</v>
@@ -3251,7 +3251,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>16</v>
@@ -3298,7 +3298,7 @@
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>16</v>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>16</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>16</v>
@@ -3439,7 +3439,7 @@
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>16</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>16</v>
@@ -3533,7 +3533,7 @@
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>16</v>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>16</v>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>16</v>
@@ -3674,7 +3674,7 @@
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>16</v>
@@ -3721,7 +3721,7 @@
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>17</v>
@@ -3768,7 +3768,7 @@
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>17</v>
@@ -3815,7 +3815,7 @@
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>17</v>
@@ -3862,7 +3862,7 @@
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>17</v>
@@ -3909,7 +3909,7 @@
     </row>
     <row r="38" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>17</v>
@@ -3956,7 +3956,7 @@
     </row>
     <row r="39" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>17</v>
@@ -4003,7 +4003,7 @@
     </row>
     <row r="40" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>17</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="41" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>17</v>
@@ -4097,7 +4097,7 @@
     </row>
     <row r="42" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>17</v>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>17</v>
@@ -4191,7 +4191,7 @@
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>17</v>
@@ -4238,7 +4238,7 @@
     </row>
     <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>17</v>
@@ -4285,7 +4285,7 @@
     </row>
     <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>17</v>
@@ -4332,7 +4332,7 @@
     </row>
     <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>17</v>
@@ -4379,7 +4379,7 @@
     </row>
     <row r="48" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>17</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
[UPDATE] Budget, Report, and Approval
</commit_message>
<xml_diff>
--- a/uploads/excel/RKAP Tempalate Fix.xlsx
+++ b/uploads/excel/RKAP Tempalate Fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Magang\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0C7CF8-DBC2-4B42-ACDE-9C09A150F199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654A05AD-239F-4851-BF45-F618F5050D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12630" yWindow="3000" windowWidth="14205" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rkap" sheetId="1" r:id="rId1"/>
@@ -2135,8 +2135,8 @@
   </sheetPr>
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2193,7 +2193,7 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
@@ -2340,7 +2340,7 @@
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>15</v>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>15</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>15</v>
@@ -2732,7 +2732,7 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
@@ -2781,7 +2781,7 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
@@ -2828,7 +2828,7 @@
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>16</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>16</v>
@@ -3063,7 +3063,7 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>16</v>
@@ -3110,7 +3110,7 @@
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>16</v>
@@ -3157,7 +3157,7 @@
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>16</v>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>16</v>
@@ -3251,7 +3251,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>16</v>
@@ -3298,7 +3298,7 @@
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>16</v>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>16</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>16</v>
@@ -3439,7 +3439,7 @@
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>16</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>16</v>
@@ -3533,7 +3533,7 @@
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>16</v>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>16</v>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>16</v>
@@ -3674,7 +3674,7 @@
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
[UPDATE] Fix Approval TXC
</commit_message>
<xml_diff>
--- a/uploads/excel/RKAP Tempalate Fix.xlsx
+++ b/uploads/excel/RKAP Tempalate Fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Magang\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD0AE2F-21B3-42AE-96D8-FB832E662D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FEE1BE-2905-4051-B44A-35DE4D1A3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1959,7 +1959,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2001,20 +2001,17 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2237,8 +2234,8 @@
   </sheetPr>
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2249,60 +2246,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="20" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B2" s="22" t="s">
+      <c r="A2" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="17">
         <v>40010001</v>
       </c>
       <c r="D2" s="18">
@@ -2345,13 +2342,13 @@
       <c r="Q2" s="6"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="17">
         <v>40012000</v>
       </c>
       <c r="D3" s="18">
@@ -2394,13 +2391,13 @@
       <c r="Q3" s="6"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B4" s="22" t="s">
+      <c r="A4" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="17">
         <v>40020001</v>
       </c>
       <c r="D4" s="18">
@@ -2443,13 +2440,13 @@
       <c r="Q4" s="7"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="17">
         <v>40014200</v>
       </c>
       <c r="D5" s="18">
@@ -2492,13 +2489,13 @@
       <c r="Q5" s="7"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="17">
         <v>40000000</v>
       </c>
       <c r="D6" s="18">
@@ -2541,13 +2538,13 @@
       <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="17">
         <v>40002002</v>
       </c>
       <c r="D7" s="18">
@@ -2590,13 +2587,13 @@
       <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B8" s="22" t="s">
+      <c r="A8" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="17">
         <v>40000400</v>
       </c>
       <c r="D8" s="18">
@@ -2639,13 +2636,13 @@
       <c r="Q8" s="7"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="17">
         <v>40000403</v>
       </c>
       <c r="D9" s="18">
@@ -2688,13 +2685,13 @@
       <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B10" s="22" t="s">
+      <c r="A10" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="17">
         <v>40030000</v>
       </c>
       <c r="D10" s="18">
@@ -2737,13 +2734,13 @@
       <c r="Q10" s="6"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B11" s="22" t="s">
+      <c r="A11" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="17">
         <v>40030001</v>
       </c>
       <c r="D11" s="18">
@@ -2786,13 +2783,13 @@
       <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="17">
         <v>40040000</v>
       </c>
       <c r="D12" s="18">
@@ -2835,13 +2832,13 @@
       <c r="Q12" s="7"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="17">
         <v>40040005</v>
       </c>
       <c r="D13" s="18">
@@ -2884,13 +2881,13 @@
       <c r="Q13" s="7"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="17">
         <v>40041002</v>
       </c>
       <c r="D14" s="18">
@@ -2931,13 +2928,13 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B15" s="22" t="s">
+      <c r="A15" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="17">
         <v>40041000</v>
       </c>
       <c r="D15" s="18">
@@ -2978,13 +2975,13 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B16" s="22" t="s">
+      <c r="A16" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="17">
         <v>40043000</v>
       </c>
       <c r="D16" s="18">
@@ -3025,13 +3022,13 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
-        <v>2023</v>
-      </c>
-      <c r="B17" s="22" t="s">
+      <c r="A17" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="17">
         <v>40043006</v>
       </c>
       <c r="D17" s="18">
@@ -3072,13 +3069,13 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B18" s="22" t="s">
+      <c r="A18" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="17">
         <v>40010001</v>
       </c>
       <c r="D18" s="18">
@@ -3119,13 +3116,13 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B19" s="22" t="s">
+      <c r="A19" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="17">
         <v>40012000</v>
       </c>
       <c r="D19" s="18">
@@ -3166,13 +3163,13 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B20" s="22" t="s">
+      <c r="A20" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="17">
         <v>40020001</v>
       </c>
       <c r="D20" s="18">
@@ -3213,13 +3210,13 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B21" s="22" t="s">
+      <c r="A21" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="17">
         <v>40014200</v>
       </c>
       <c r="D21" s="18">
@@ -3260,13 +3257,13 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="17">
         <v>40000000</v>
       </c>
       <c r="D22" s="18">
@@ -3307,13 +3304,13 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B23" s="22" t="s">
+      <c r="A23" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="17">
         <v>40002002</v>
       </c>
       <c r="D23" s="18">
@@ -3354,13 +3351,13 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B24" s="22" t="s">
+      <c r="A24" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="17">
         <v>40000400</v>
       </c>
       <c r="D24" s="18">
@@ -3401,13 +3398,13 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B25" s="22" t="s">
+      <c r="A25" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="17">
         <v>40000403</v>
       </c>
       <c r="D25" s="18">
@@ -3448,13 +3445,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B26" s="22" t="s">
+      <c r="A26" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="17">
         <v>40030000</v>
       </c>
       <c r="D26" s="18">
@@ -3495,13 +3492,13 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B27" s="22" t="s">
+      <c r="A27" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="17">
         <v>40030001</v>
       </c>
       <c r="D27" s="18">
@@ -3542,13 +3539,13 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B28" s="22" t="s">
+      <c r="A28" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="17">
         <v>40040000</v>
       </c>
       <c r="D28" s="18">
@@ -3589,13 +3586,13 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B29" s="22" t="s">
+      <c r="A29" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B29" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="17">
         <v>40040005</v>
       </c>
       <c r="D29" s="18">
@@ -3636,13 +3633,13 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B30" s="22" t="s">
+      <c r="A30" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B30" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30" s="17">
         <v>40041002</v>
       </c>
       <c r="D30" s="18">
@@ -3683,13 +3680,13 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B31" s="22" t="s">
+      <c r="A31" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="17">
         <v>40041000</v>
       </c>
       <c r="D31" s="18">
@@ -3730,13 +3727,13 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B32" s="22" t="s">
+      <c r="A32" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32" s="17">
         <v>40043000</v>
       </c>
       <c r="D32" s="18">
@@ -3777,13 +3774,13 @@
       </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22">
-        <v>2022</v>
-      </c>
-      <c r="B33" s="22" t="s">
+      <c r="A33" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="17">
         <v>40043006</v>
       </c>
       <c r="D33" s="18">
@@ -3824,13 +3821,13 @@
       </c>
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B34" s="22" t="s">
+      <c r="A34" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="22">
+      <c r="C34" s="17">
         <v>40010001</v>
       </c>
       <c r="D34" s="18">
@@ -3871,13 +3868,13 @@
       </c>
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B35" s="22" t="s">
+      <c r="A35" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="17">
         <v>40012000</v>
       </c>
       <c r="D35" s="18">
@@ -3918,13 +3915,13 @@
       </c>
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B36" s="22" t="s">
+      <c r="A36" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="22">
+      <c r="C36" s="17">
         <v>40020001</v>
       </c>
       <c r="D36" s="18">
@@ -3965,13 +3962,13 @@
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B37" s="22" t="s">
+      <c r="A37" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="22">
+      <c r="C37" s="17">
         <v>40014200</v>
       </c>
       <c r="D37" s="18">
@@ -4012,13 +4009,13 @@
       </c>
     </row>
     <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B38" s="22" t="s">
+      <c r="A38" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B38" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="22">
+      <c r="C38" s="17">
         <v>40000000</v>
       </c>
       <c r="D38" s="18">
@@ -4059,13 +4056,13 @@
       </c>
     </row>
     <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B39" s="22" t="s">
+      <c r="A39" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B39" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="22">
+      <c r="C39" s="17">
         <v>40002002</v>
       </c>
       <c r="D39" s="18">
@@ -4106,13 +4103,13 @@
       </c>
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B40" s="22" t="s">
+      <c r="A40" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B40" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="22">
+      <c r="C40" s="17">
         <v>40000400</v>
       </c>
       <c r="D40" s="18">
@@ -4153,13 +4150,13 @@
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B41" s="22" t="s">
+      <c r="A41" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B41" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="22">
+      <c r="C41" s="17">
         <v>40000403</v>
       </c>
       <c r="D41" s="18">
@@ -4200,13 +4197,13 @@
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B42" s="22" t="s">
+      <c r="A42" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B42" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="22">
+      <c r="C42" s="17">
         <v>40030000</v>
       </c>
       <c r="D42" s="18">
@@ -4247,13 +4244,13 @@
       </c>
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B43" s="22" t="s">
+      <c r="A43" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="22">
+      <c r="C43" s="17">
         <v>40030001</v>
       </c>
       <c r="D43" s="18">
@@ -4294,13 +4291,13 @@
       </c>
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B44" s="22" t="s">
+      <c r="A44" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B44" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="22">
+      <c r="C44" s="17">
         <v>40040000</v>
       </c>
       <c r="D44" s="18">
@@ -4341,13 +4338,13 @@
       </c>
     </row>
     <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B45" s="22" t="s">
+      <c r="A45" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B45" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="22">
+      <c r="C45" s="17">
         <v>40040005</v>
       </c>
       <c r="D45" s="18">
@@ -4388,13 +4385,13 @@
       </c>
     </row>
     <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B46" s="22" t="s">
+      <c r="A46" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B46" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="22">
+      <c r="C46" s="17">
         <v>40041002</v>
       </c>
       <c r="D46" s="18">
@@ -4435,13 +4432,13 @@
       </c>
     </row>
     <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B47" s="22" t="s">
+      <c r="A47" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B47" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="17">
         <v>40041000</v>
       </c>
       <c r="D47" s="18">
@@ -4482,13 +4479,13 @@
       </c>
     </row>
     <row r="48" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B48" s="22" t="s">
+      <c r="A48" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B48" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C48" s="22">
+      <c r="C48" s="17">
         <v>40043000</v>
       </c>
       <c r="D48" s="18">
@@ -4529,13 +4526,13 @@
       </c>
     </row>
     <row r="49" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22">
-        <v>2021</v>
-      </c>
-      <c r="B49" s="23" t="s">
+      <c r="A49" s="17">
+        <v>2024</v>
+      </c>
+      <c r="B49" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="22">
+      <c r="C49" s="17">
         <v>40043006</v>
       </c>
       <c r="D49" s="18">
@@ -11804,10 +11801,10 @@
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="19"/>
+      <c r="B55" s="22"/>
       <c r="C55" s="8">
         <f t="shared" si="23"/>
         <v>132242</v>

</xml_diff>